<commit_message>
Doan Day danh sach loi toi 08/04/2019
</commit_message>
<xml_diff>
--- a/Document/5.Reference/1.Server_Info.xlsx
+++ b/Document/5.Reference/1.Server_Info.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49158E36-ED03-42F3-A896-0E5F4717CE44}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1BB781D-05DA-4582-8DB5-FC227A9102AE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="20" windowWidth="19180" windowHeight="10180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="380" windowWidth="19180" windowHeight="10180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -442,7 +442,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -508,7 +508,7 @@
       <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="1"/>
@@ -650,8 +650,9 @@
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{03F389F7-283E-4B85-B9EB-177200338CC3}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{B1E57911-36DC-45AD-8589-D7FC25CBD04C}"/>
+    <hyperlink ref="E3" r:id="rId3" xr:uid="{5223E99C-7AC2-4553-9465-E93BCAD29B5D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>